<commit_message>
feat: Implement Advanced DSL Validation and AI Healer Confidence Scoring
</commit_message>
<xml_diff>
--- a/data-vault/data/test-suite.xlsx
+++ b/data-vault/data/test-suite.xlsx
@@ -397,56 +397,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>testCaseId</v>
+      </c>
+      <c r="B1" t="str">
         <v>id</v>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>action</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>selector</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>data</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>TC001</v>
+      </c>
+      <c r="B2" t="str">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>navigate</v>
       </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
       <c r="D2" t="str">
-        <v>https://testplacementwebv1.azurewebsites.net/</v>
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v>HOME_PAGE</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>TC001</v>
+      </c>
+      <c r="B3" t="str">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
+        <v>click</v>
+      </c>
+      <c r="D3" t="str">
+        <v>EMPLOYER_PORTAL_BTN</v>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>TC001</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
         <v>waitFor</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D4" t="str">
+        <v>WELCOME_HEADER</v>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>TC002</v>
+      </c>
+      <c r="B5" t="str">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <v>navigate</v>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v>https://google.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>TC002</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2</v>
+      </c>
+      <c r="C6" t="str">
+        <v>waitFor</v>
+      </c>
+      <c r="D6" t="str">
         <v>body</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>TC003</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <v>navigate</v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v>HOME_PAGE</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>TC003</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2</v>
+      </c>
+      <c r="C8" t="str">
+        <v>click</v>
+      </c>
+      <c r="D8" t="str">
+        <v>EMPLOYER_PORTAL_BTN</v>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>TC003</v>
+      </c>
+      <c r="B9" t="str">
+        <v>3</v>
+      </c>
+      <c r="C9" t="str">
+        <v>click</v>
+      </c>
+      <c r="D9" t="str">
+        <v>EMPLOYER_LOGIN_BTN</v>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>TC003</v>
+      </c>
+      <c r="B10" t="str">
+        <v>4</v>
+      </c>
+      <c r="C10" t="str">
+        <v>waitFor</v>
+      </c>
+      <c r="D10" t="str">
+        <v>text=Invalid</v>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B11" t="str">
+        <v>1</v>
+      </c>
+      <c r="C11" t="str">
+        <v>LOGIN_TO_EMPLOYER_PORTAL</v>
+      </c>
+      <c r="D11" t="str">
+        <v/>
+      </c>
+      <c r="E11" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: implement strict mode and resilient clicking for TC004 stability
</commit_message>
<xml_diff>
--- a/data-vault/data/test-suite.xlsx
+++ b/data-vault/data/test-suite.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -580,18 +580,171 @@
         <v>1</v>
       </c>
       <c r="C11" t="str">
-        <v>LOGIN_TO_EMPLOYER_PORTAL</v>
+        <v>navigate</v>
       </c>
       <c r="D11" t="str">
         <v/>
       </c>
       <c r="E11" t="str">
+        <v>https://testplacementwebv1.azurewebsites.net/</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2</v>
+      </c>
+      <c r="C12" t="str">
+        <v>click</v>
+      </c>
+      <c r="D12" t="str">
+        <v>css:a[href*='logType=EMP']</v>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B13" t="str">
+        <v>3</v>
+      </c>
+      <c r="C13" t="str">
+        <v>waitFor</v>
+      </c>
+      <c r="D13" t="str">
+        <v>css:button:has-text('Employer Login')</v>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B14" t="str">
+        <v>4</v>
+      </c>
+      <c r="C14" t="str">
+        <v>click</v>
+      </c>
+      <c r="D14" t="str">
+        <v>css:button:has-text('Employer Login')</v>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B15" t="str">
+        <v>5</v>
+      </c>
+      <c r="C15" t="str">
+        <v>click</v>
+      </c>
+      <c r="D15" t="str">
+        <v>css:button:has-text('Sign in with email')</v>
+      </c>
+      <c r="E15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B16" t="str">
+        <v>6</v>
+      </c>
+      <c r="C16" t="str">
+        <v>type</v>
+      </c>
+      <c r="D16" t="str">
+        <v>css:input[name='email']</v>
+      </c>
+      <c r="E16" t="str">
+        <v>oracle.tech@yopmail.com</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B17" t="str">
+        <v>7</v>
+      </c>
+      <c r="C17" t="str">
+        <v>click</v>
+      </c>
+      <c r="D17" t="str">
+        <v>css:button:has-text('Next')</v>
+      </c>
+      <c r="E17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B18" t="str">
+        <v>8</v>
+      </c>
+      <c r="C18" t="str">
+        <v>type</v>
+      </c>
+      <c r="D18" t="str">
+        <v>css:input[name='password']</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Pibm@123</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B19" t="str">
+        <v>9</v>
+      </c>
+      <c r="C19" t="str">
+        <v>click</v>
+      </c>
+      <c r="D19" t="str">
+        <v>css:button:has-text('Sign In')</v>
+      </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>TC004</v>
+      </c>
+      <c r="B20" t="str">
+        <v>10</v>
+      </c>
+      <c r="C20" t="str">
+        <v>waitFor</v>
+      </c>
+      <c r="D20" t="str">
+        <v>text=Dashboard</v>
+      </c>
+      <c r="E20" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>